<commit_message>
EEE faculty excel formatted
</commit_message>
<xml_diff>
--- a/Modified Data/EEE/EEE1.xlsx
+++ b/Modified Data/EEE/EEE1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VLSID\Mukesh\Time_Table_Management_Using_GenAI\Modified Data\EEE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE9F6A51-CFE9-4F50-8C2E-651119BCF01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F84114-D761-411D-88AC-553C803C84AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11295" xr2:uid="{7E6DE806-A961-4CB0-BBFB-AF529762BAC5}"/>
   </bookViews>
@@ -380,13 +380,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -452,6 +445,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -547,111 +548,110 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -971,1065 +971,1065 @@
   <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="9.140625" style="45"/>
+    <col min="3" max="3" width="9.140625" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="39.75" thickBot="1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="39.75" thickBot="1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="39.75" thickBot="1">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="39.75" thickBot="1">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="39.75" thickBot="1">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="39.75" thickBot="1">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="27" thickBot="1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="60.75" thickBot="1">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="60.75" thickBot="1">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="E14" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60.75" thickBot="1">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="E17" s="16" t="s">
+      <c r="E17" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="24" t="s">
+      <c r="D18" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="60.75" thickBot="1">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="13" t="s">
+      <c r="D22" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="39.75" thickBot="1">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E26" s="21" t="s">
+      <c r="E26" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="39.75" thickBot="1">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="D27" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="27" thickBot="1">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="26" t="s">
+      <c r="D28" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E28" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="27" thickBot="1">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E29" s="21" t="s">
+      <c r="E29" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="14" t="s">
+      <c r="D30" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30.75" thickBot="1">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="D31" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="16" t="s">
+      <c r="E31" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="7" t="s">
+      <c r="C32" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="14" t="s">
+      <c r="D32" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="39.75" thickBot="1">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="26" t="s">
+      <c r="D34" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="39.75" thickBot="1">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D35" s="26" t="s">
+      <c r="D35" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D36" s="27" t="s">
+      <c r="D36" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="45.75" thickBot="1">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="27" t="s">
+      <c r="D37" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="E37" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="39.75" thickBot="1">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D38" s="11" t="s">
+      <c r="D38" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="25" t="s">
+      <c r="E38" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="39.75" thickBot="1">
-      <c r="A39" s="17" t="s">
+      <c r="A39" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E39" s="21" t="s">
+      <c r="E39" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="27" thickBot="1">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C40" s="43" t="s">
+      <c r="C40" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="C41" s="43" t="s">
+      <c r="C41" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D41" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="E41" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:5" ht="27" thickBot="1">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B42" s="29" t="s">
+      <c r="B42" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="43" t="s">
+      <c r="C42" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="27" thickBot="1">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="C43" s="43" t="s">
+      <c r="C43" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="43" t="s">
+      <c r="C44" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D44" s="31" t="s">
+      <c r="D44" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C45" s="43" t="s">
+      <c r="C45" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="31" t="s">
+      <c r="D45" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C46" s="43" t="s">
+      <c r="C46" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="D46" s="31" t="s">
+      <c r="D46" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E46" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="C47" s="43" t="s">
+      <c r="C47" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="D47" s="31" t="s">
+      <c r="D47" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="E47" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="43" t="s">
+      <c r="C48" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="31" t="s">
+      <c r="D48" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="E48" s="25" t="s">
+      <c r="E48" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B49" s="29" t="s">
+      <c r="B49" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="C49" s="43" t="s">
+      <c r="C49" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="D49" s="31" t="s">
+      <c r="D49" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="E49" s="21" t="s">
+      <c r="E49" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B50" s="29" t="s">
+      <c r="B50" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C50" s="43" t="s">
+      <c r="C50" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="D50" s="31" t="s">
+      <c r="D50" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E50" s="16" t="s">
+      <c r="E50" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="C51" s="43" t="s">
+      <c r="C51" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="D51" s="31" t="s">
+      <c r="D51" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E51" s="16" t="s">
+      <c r="E51" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B52" s="29" t="s">
+      <c r="B52" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="C52" s="43" t="s">
+      <c r="C52" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="D52" s="31" t="s">
+      <c r="D52" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E52" s="15" t="s">
+      <c r="E52" s="14" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="C53" s="43" t="s">
+      <c r="C53" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="D53" s="31" t="s">
+      <c r="D53" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E53" s="14" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A54" s="17" t="s">
+      <c r="A54" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C54" s="43" t="s">
+      <c r="C54" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="D54" s="32" t="s">
+      <c r="D54" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="E54" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A55" s="17" t="s">
+      <c r="A55" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="C55" s="43" t="s">
+      <c r="C55" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="D55" s="32" t="s">
+      <c r="D55" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="E55" s="16" t="s">
+      <c r="E55" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A56" s="17" t="s">
+      <c r="A56" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="29" t="s">
+      <c r="B56" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C56" s="43" t="s">
+      <c r="C56" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D56" s="33" t="s">
+      <c r="D56" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="E56" s="16" t="s">
+      <c r="E56" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A57" s="34" t="s">
+      <c r="A57" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="B57" s="29" t="s">
+      <c r="B57" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="C57" s="43" t="s">
+      <c r="C57" s="42" t="s">
         <v>87</v>
       </c>
-      <c r="D57" s="33" t="s">
+      <c r="D57" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="E57" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B58" s="35" t="s">
+      <c r="B58" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="C58" s="46" t="s">
+      <c r="C58" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="D58" s="36" t="s">
+      <c r="D58" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="E58" s="37" t="s">
+      <c r="E58" s="36" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B59" s="38" t="s">
+      <c r="B59" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="C59" s="44" t="s">
+      <c r="C59" s="43" t="s">
         <v>94</v>
       </c>
-      <c r="D59" s="36" t="s">
+      <c r="D59" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="E59" s="39" t="s">
+      <c r="E59" s="38" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B60" s="38" t="s">
+      <c r="B60" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="C60" s="43" t="s">
+      <c r="C60" s="42" t="s">
         <v>96</v>
       </c>
-      <c r="D60" s="36" t="s">
+      <c r="D60" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="E60" s="37" t="s">
+      <c r="E60" s="36" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B61" s="38" t="s">
+      <c r="B61" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="C61" s="43" t="s">
+      <c r="C61" s="42" t="s">
         <v>99</v>
       </c>
-      <c r="D61" s="36" t="s">
+      <c r="D61" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="E61" s="40" t="s">
+      <c r="E61" s="39" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B62" s="38" t="s">
+      <c r="B62" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="C62" s="43" t="s">
+      <c r="C62" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="D62" s="36" t="s">
+      <c r="D62" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="E62" s="39" t="s">
+      <c r="E62" s="38" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>